<commit_message>
Primeira coverage do Duf
</commit_message>
<xml_diff>
--- a/data-raw/cliente-duf/42519_Tabela MMA 27.04.xlsx
+++ b/data-raw/cliente-duf/42519_Tabela MMA 27.04.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20344"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueShift075\Documents\GitHub\Intelipost-Media\data-raw\cliente-duf\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291F7134-BA0F-4AE1-9907-900505C5483A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -640,12 +646,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="_(&quot;R$ &quot;* #,##0.00_);_(&quot;R$ &quot;* \(#,##0.00\);_(&quot;R$ &quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1094,13 +1100,21 @@
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
-    <cellStyle name="Moeda 2" xfId="2"/>
+    <cellStyle name="Moeda 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1114,8 +1128,8 @@
       <xdr:rowOff>56026</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>134470</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>217020</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>156879</xdr:rowOff>
     </xdr:to>
@@ -1124,7 +1138,7 @@
         <xdr:cNvPr id="2" name="Imagem 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FAA27946-2A6E-482E-915B-F99E5013305E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAA27946-2A6E-482E-915B-F99E5013305E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1136,7 +1150,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1156,7 +1170,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1171,9 +1185,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1211,9 +1225,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1245,9 +1259,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1279,9 +1311,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1454,22 +1504,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A6:L68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A26" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="10" max="10" width="11.7265625" customWidth="1"/>
+    <col min="11" max="11" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
@@ -1492,7 +1543,7 @@
       </c>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="16.5">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>4</v>
       </c>
@@ -1507,7 +1558,7 @@
       <c r="J7" s="5"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" ht="16.5">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="52"/>
       <c r="B8" s="52"/>
       <c r="C8" s="53"/>
@@ -1520,7 +1571,7 @@
       <c r="J8" s="57"/>
       <c r="K8" s="58"/>
     </row>
-    <row r="9" spans="1:11" ht="16.5">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="59"/>
       <c r="B9" s="59"/>
       <c r="C9" s="60"/>
@@ -1533,7 +1584,7 @@
       <c r="J9" s="64"/>
       <c r="K9" s="65"/>
     </row>
-    <row r="10" spans="1:11" ht="16.5">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="68" t="s">
         <v>5</v>
       </c>
@@ -1556,7 +1607,7 @@
       <c r="J10" s="6"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="68"/>
       <c r="B11" s="22"/>
       <c r="C11" s="71"/>
@@ -1573,7 +1624,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1590,7 +1641,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" ht="16.5">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="28"/>
@@ -1603,7 +1654,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="27" t="s">
         <v>14</v>
       </c>
@@ -1618,7 +1669,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="27" t="s">
         <v>15</v>
       </c>
@@ -1633,7 +1684,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="30">
+    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="44" t="s">
         <v>16</v>
       </c>
@@ -1656,7 +1707,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="45" t="s">
         <v>21</v>
       </c>
@@ -1680,7 +1731,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="45" t="s">
         <v>21</v>
       </c>
@@ -1704,7 +1755,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="45" t="s">
         <v>24</v>
       </c>
@@ -1728,7 +1779,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="45" t="s">
         <v>24</v>
       </c>
@@ -1752,7 +1803,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="69"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="45" t="s">
         <v>26</v>
       </c>
@@ -1776,7 +1827,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="45" t="s">
         <v>26</v>
       </c>
@@ -1800,7 +1851,7 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75">
+    <row r="24" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="36" t="s">
         <v>28</v>
       </c>
@@ -1816,7 +1867,7 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="29" t="s">
         <v>29</v>
       </c>
@@ -1834,7 +1885,7 @@
       </c>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="31" t="s">
         <v>30</v>
       </c>
@@ -1852,7 +1903,7 @@
       </c>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="33" t="s">
         <v>32</v>
       </c>
@@ -1870,7 +1921,7 @@
       </c>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="33" t="s">
         <v>33</v>
       </c>
@@ -1888,7 +1939,7 @@
       </c>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="33" t="s">
         <v>34</v>
       </c>
@@ -1906,7 +1957,7 @@
       </c>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="33" t="s">
         <v>35</v>
       </c>
@@ -1922,7 +1973,7 @@
       <c r="K31" s="50"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="33" t="s">
         <v>36</v>
       </c>
@@ -1940,7 +1991,7 @@
       </c>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="31" t="s">
         <v>38</v>
       </c>
@@ -1957,7 +2008,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="33" t="s">
         <v>39</v>
       </c>
@@ -1974,7 +2025,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="29" t="s">
         <v>41</v>
       </c>
@@ -1991,7 +2042,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="34" t="s">
         <v>42</v>
       </c>
@@ -2008,7 +2059,7 @@
         <v>208.4</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="34" t="s">
         <v>43</v>
       </c>
@@ -2025,7 +2076,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="34" t="s">
         <v>44</v>
       </c>
@@ -2040,7 +2091,7 @@
       <c r="J38" s="34"/>
       <c r="K38" s="34"/>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="31" t="s">
         <v>45</v>
       </c>
@@ -2055,7 +2106,7 @@
       <c r="J39" s="31"/>
       <c r="K39" s="31"/>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="29" t="s">
         <v>46</v>
       </c>
@@ -2070,7 +2121,7 @@
       <c r="J40" s="29"/>
       <c r="K40" s="29"/>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="31" t="s">
         <v>47</v>
       </c>
@@ -2087,7 +2138,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="39" t="s">
         <v>48</v>
       </c>
@@ -2104,7 +2155,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="41" t="s">
         <v>49</v>
       </c>
@@ -2121,7 +2172,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="42" t="s">
         <v>50</v>
       </c>
@@ -2138,7 +2189,7 @@
         <v>15.73</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="39" t="s">
         <v>51</v>
       </c>
@@ -2155,7 +2206,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="39" t="s">
         <v>52</v>
       </c>
@@ -2172,7 +2223,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="39" t="s">
         <v>53</v>
       </c>
@@ -2189,7 +2240,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="39" t="s">
         <v>54</v>
       </c>
@@ -2206,7 +2257,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="41" t="s">
         <v>55</v>
       </c>
@@ -2221,7 +2272,7 @@
       <c r="J49" s="29"/>
       <c r="K49" s="29"/>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="42" t="s">
         <v>56</v>
       </c>
@@ -2238,7 +2289,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="42" t="s">
         <v>57</v>
       </c>
@@ -2255,7 +2306,7 @@
       </c>
       <c r="K51" s="33"/>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" s="78" t="s">
         <v>59</v>
       </c>
@@ -2272,7 +2323,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="39" t="s">
         <v>60</v>
       </c>
@@ -2287,7 +2338,7 @@
       <c r="J53" s="33"/>
       <c r="K53" s="33"/>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" s="37" t="s">
         <v>61</v>
       </c>
@@ -2302,7 +2353,7 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="81" t="s">
         <v>62</v>
       </c>
@@ -2317,7 +2368,7 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" s="29" t="s">
         <v>63</v>
       </c>
@@ -2332,7 +2383,7 @@
       <c r="J56" s="29"/>
       <c r="K56" s="29"/>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="31" t="s">
         <v>64</v>
       </c>
@@ -2347,7 +2398,7 @@
       <c r="J57" s="31"/>
       <c r="K57" s="31"/>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" s="33" t="s">
         <v>65</v>
       </c>
@@ -2362,7 +2413,7 @@
       <c r="J58" s="33"/>
       <c r="K58" s="33"/>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="33" t="s">
         <v>66</v>
       </c>
@@ -2377,7 +2428,7 @@
       <c r="J59" s="33"/>
       <c r="K59" s="33"/>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="29" t="s">
         <v>67</v>
       </c>
@@ -2392,7 +2443,7 @@
       <c r="J60" s="29"/>
       <c r="K60" s="29"/>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="31" t="s">
         <v>68</v>
       </c>
@@ -2407,7 +2458,7 @@
       <c r="J61" s="31"/>
       <c r="K61" s="31"/>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" s="29" t="s">
         <v>69</v>
       </c>
@@ -2422,7 +2473,7 @@
       <c r="J62" s="29"/>
       <c r="K62" s="29"/>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" s="31" t="s">
         <v>70</v>
       </c>
@@ -2437,7 +2488,7 @@
       <c r="J63" s="31"/>
       <c r="K63" s="31"/>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" s="80"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2450,7 +2501,7 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>71</v>
       </c>
@@ -2465,7 +2516,7 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2480,7 +2531,7 @@
       <c r="J66" s="67"/>
       <c r="K66" s="67"/>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>73</v>
       </c>
@@ -2497,7 +2548,7 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>75</v>
       </c>
@@ -2514,33 +2565,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I12" r:id="rId1"/>
+    <hyperlink ref="I12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" scale="71" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="71" orientation="portrait" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Carga fracionada xlsx (Onofre)
Revisão de alguns códigos visando torná-los mais robustos a variações de entrada e início da preparação do cenário de carga fracionada com entradas em xlsx.
</commit_message>
<xml_diff>
--- a/data-raw/cliente-duf/42519_Tabela MMA 27.04.xlsx
+++ b/data-raw/cliente-duf/42519_Tabela MMA 27.04.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20344"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueShift075\Documents\GitHub\Intelipost-Media\data-raw\cliente-duf\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291F7134-BA0F-4AE1-9907-900505C5483A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -646,12 +640,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="_(&quot;R$ &quot;* #,##0.00_);_(&quot;R$ &quot;* \(#,##0.00\);_(&quot;R$ &quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1100,21 +1094,13 @@
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
-    <cellStyle name="Moeda 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Moeda 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1128,8 +1114,8 @@
       <xdr:rowOff>56026</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>217020</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>134470</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>156879</xdr:rowOff>
     </xdr:to>
@@ -1138,7 +1124,7 @@
         <xdr:cNvPr id="2" name="Imagem 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAA27946-2A6E-482E-915B-F99E5013305E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FAA27946-2A6E-482E-915B-F99E5013305E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1150,7 +1136,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1170,7 +1156,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1185,9 +1171,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1225,9 +1211,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1259,27 +1245,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1311,27 +1279,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1504,23 +1454,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A6:L68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A26" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
-    <col min="10" max="10" width="11.7265625" customWidth="1"/>
-    <col min="11" max="11" width="13.7265625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11">
       <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
@@ -1543,7 +1492,7 @@
       </c>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="16.5">
       <c r="A7" s="13" t="s">
         <v>4</v>
       </c>
@@ -1558,7 +1507,7 @@
       <c r="J7" s="5"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="16.5">
       <c r="A8" s="52"/>
       <c r="B8" s="52"/>
       <c r="C8" s="53"/>
@@ -1571,7 +1520,7 @@
       <c r="J8" s="57"/>
       <c r="K8" s="58"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="16.5">
       <c r="A9" s="59"/>
       <c r="B9" s="59"/>
       <c r="C9" s="60"/>
@@ -1584,7 +1533,7 @@
       <c r="J9" s="64"/>
       <c r="K9" s="65"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="16.5">
       <c r="A10" s="68" t="s">
         <v>5</v>
       </c>
@@ -1607,7 +1556,7 @@
       <c r="J10" s="6"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" s="68"/>
       <c r="B11" s="22"/>
       <c r="C11" s="71"/>
@@ -1624,7 +1573,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1641,7 +1590,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="16.5">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="28"/>
@@ -1654,7 +1603,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11">
       <c r="A14" s="27" t="s">
         <v>14</v>
       </c>
@@ -1669,7 +1618,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11">
       <c r="A15" s="27" t="s">
         <v>15</v>
       </c>
@@ -1684,7 +1633,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="30">
       <c r="A16" s="44" t="s">
         <v>16</v>
       </c>
@@ -1707,7 +1656,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12">
       <c r="A17" s="45" t="s">
         <v>21</v>
       </c>
@@ -1731,7 +1680,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12">
       <c r="A18" s="45" t="s">
         <v>21</v>
       </c>
@@ -1755,7 +1704,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12">
       <c r="A19" s="45" t="s">
         <v>24</v>
       </c>
@@ -1779,7 +1728,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12">
       <c r="A20" s="45" t="s">
         <v>24</v>
       </c>
@@ -1803,7 +1752,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="69"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12">
       <c r="A21" s="45" t="s">
         <v>26</v>
       </c>
@@ -1827,7 +1776,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12">
       <c r="A22" s="45" t="s">
         <v>26</v>
       </c>
@@ -1851,7 +1800,7 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="24" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="15.75">
       <c r="A24" s="36" t="s">
         <v>28</v>
       </c>
@@ -1867,7 +1816,7 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12">
       <c r="A26" s="29" t="s">
         <v>29</v>
       </c>
@@ -1885,7 +1834,7 @@
       </c>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12">
       <c r="A27" s="31" t="s">
         <v>30</v>
       </c>
@@ -1903,7 +1852,7 @@
       </c>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12">
       <c r="A28" s="33" t="s">
         <v>32</v>
       </c>
@@ -1921,7 +1870,7 @@
       </c>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12">
       <c r="A29" s="33" t="s">
         <v>33</v>
       </c>
@@ -1939,7 +1888,7 @@
       </c>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12">
       <c r="A30" s="33" t="s">
         <v>34</v>
       </c>
@@ -1957,7 +1906,7 @@
       </c>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12">
       <c r="A31" s="33" t="s">
         <v>35</v>
       </c>
@@ -1973,7 +1922,7 @@
       <c r="K31" s="50"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12">
       <c r="A32" s="33" t="s">
         <v>36</v>
       </c>
@@ -1991,7 +1940,7 @@
       </c>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11">
       <c r="A33" s="31" t="s">
         <v>38</v>
       </c>
@@ -2008,7 +1957,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11">
       <c r="A34" s="33" t="s">
         <v>39</v>
       </c>
@@ -2025,7 +1974,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11">
       <c r="A35" s="29" t="s">
         <v>41</v>
       </c>
@@ -2042,7 +1991,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11">
       <c r="A36" s="34" t="s">
         <v>42</v>
       </c>
@@ -2059,7 +2008,7 @@
         <v>208.4</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11">
       <c r="A37" s="34" t="s">
         <v>43</v>
       </c>
@@ -2076,7 +2025,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11">
       <c r="A38" s="34" t="s">
         <v>44</v>
       </c>
@@ -2091,7 +2040,7 @@
       <c r="J38" s="34"/>
       <c r="K38" s="34"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11">
       <c r="A39" s="31" t="s">
         <v>45</v>
       </c>
@@ -2106,7 +2055,7 @@
       <c r="J39" s="31"/>
       <c r="K39" s="31"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11">
       <c r="A40" s="29" t="s">
         <v>46</v>
       </c>
@@ -2121,7 +2070,7 @@
       <c r="J40" s="29"/>
       <c r="K40" s="29"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11">
       <c r="A41" s="31" t="s">
         <v>47</v>
       </c>
@@ -2138,7 +2087,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11">
       <c r="A42" s="39" t="s">
         <v>48</v>
       </c>
@@ -2155,7 +2104,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11">
       <c r="A43" s="41" t="s">
         <v>49</v>
       </c>
@@ -2172,7 +2121,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11">
       <c r="A44" s="42" t="s">
         <v>50</v>
       </c>
@@ -2189,7 +2138,7 @@
         <v>15.73</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11">
       <c r="A45" s="39" t="s">
         <v>51</v>
       </c>
@@ -2206,7 +2155,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11">
       <c r="A46" s="39" t="s">
         <v>52</v>
       </c>
@@ -2223,7 +2172,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11">
       <c r="A47" s="39" t="s">
         <v>53</v>
       </c>
@@ -2240,7 +2189,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11">
       <c r="A48" s="39" t="s">
         <v>54</v>
       </c>
@@ -2257,7 +2206,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11">
       <c r="A49" s="41" t="s">
         <v>55</v>
       </c>
@@ -2272,7 +2221,7 @@
       <c r="J49" s="29"/>
       <c r="K49" s="29"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11">
       <c r="A50" s="42" t="s">
         <v>56</v>
       </c>
@@ -2289,7 +2238,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11">
       <c r="A51" s="42" t="s">
         <v>57</v>
       </c>
@@ -2306,7 +2255,7 @@
       </c>
       <c r="K51" s="33"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11">
       <c r="A52" s="78" t="s">
         <v>59</v>
       </c>
@@ -2323,7 +2272,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11">
       <c r="A53" s="39" t="s">
         <v>60</v>
       </c>
@@ -2338,7 +2287,7 @@
       <c r="J53" s="33"/>
       <c r="K53" s="33"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11">
       <c r="A54" s="37" t="s">
         <v>61</v>
       </c>
@@ -2353,7 +2302,7 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11">
       <c r="A55" s="81" t="s">
         <v>62</v>
       </c>
@@ -2368,7 +2317,7 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11">
       <c r="A56" s="29" t="s">
         <v>63</v>
       </c>
@@ -2383,7 +2332,7 @@
       <c r="J56" s="29"/>
       <c r="K56" s="29"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11">
       <c r="A57" s="31" t="s">
         <v>64</v>
       </c>
@@ -2398,7 +2347,7 @@
       <c r="J57" s="31"/>
       <c r="K57" s="31"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11">
       <c r="A58" s="33" t="s">
         <v>65</v>
       </c>
@@ -2413,7 +2362,7 @@
       <c r="J58" s="33"/>
       <c r="K58" s="33"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11">
       <c r="A59" s="33" t="s">
         <v>66</v>
       </c>
@@ -2428,7 +2377,7 @@
       <c r="J59" s="33"/>
       <c r="K59" s="33"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11">
       <c r="A60" s="29" t="s">
         <v>67</v>
       </c>
@@ -2443,7 +2392,7 @@
       <c r="J60" s="29"/>
       <c r="K60" s="29"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11">
       <c r="A61" s="31" t="s">
         <v>68</v>
       </c>
@@ -2458,7 +2407,7 @@
       <c r="J61" s="31"/>
       <c r="K61" s="31"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11">
       <c r="A62" s="29" t="s">
         <v>69</v>
       </c>
@@ -2473,7 +2422,7 @@
       <c r="J62" s="29"/>
       <c r="K62" s="29"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11">
       <c r="A63" s="31" t="s">
         <v>70</v>
       </c>
@@ -2488,7 +2437,7 @@
       <c r="J63" s="31"/>
       <c r="K63" s="31"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11">
       <c r="A64" s="80"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2501,7 +2450,7 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11">
       <c r="A65" s="1" t="s">
         <v>71</v>
       </c>
@@ -2516,7 +2465,7 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2531,7 +2480,7 @@
       <c r="J66" s="67"/>
       <c r="K66" s="67"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11">
       <c r="A67" s="1" t="s">
         <v>73</v>
       </c>
@@ -2548,7 +2497,7 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11">
       <c r="A68" s="1" t="s">
         <v>75</v>
       </c>
@@ -2565,33 +2514,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I12" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" scale="71" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="71" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>